<commit_message>
bunch of barn files and images
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240AE747-CB2E-B448-8835-16B7E31FE4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7812E86E-5B8B-2347-A6BB-747B9225FAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>HTML</t>
   </si>
@@ -108,6 +108,90 @@
   </si>
   <si>
     <t>b-bertje.jpeg</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501210627im_/http://dewey.rug.ac.be/barn/tex/gold.html</t>
+  </si>
+  <si>
+    <t>claemit</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990428110805im_/http://dewey.rug.ac.be/barn/tex/claemit.html</t>
+  </si>
+  <si>
+    <t>theresa</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501233653im_/http://dewey.rug.ac.be/barn/tex/theresa.html</t>
+  </si>
+  <si>
+    <t>nuns</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501230557im_/http://dewey.rug.ac.be/barn/tex/nuns.html</t>
+  </si>
+  <si>
+    <t>fiat</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501204011im_/http://dewey.rug.ac.be/barn/tex/fiat.html</t>
+  </si>
+  <si>
+    <t>dildo</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501200351im_/http://dewey.rug.ac.be/barn/tex/dildo.html</t>
+  </si>
+  <si>
+    <t>meno</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501221035im_/http://dewey.rug.ac.be/barn/tex/meno.html</t>
+  </si>
+  <si>
+    <t>herma</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501213417im_/http://dewey.rug.ac.be/barn/tex/herma.html</t>
+  </si>
+  <si>
+    <t>doppler</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990501202926im_/http://dewey.rug.ac.be/barn/tex/doppler.html</t>
+  </si>
+  <si>
+    <t>piet</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990220101839im_/http://dewey.rug.ac.be/barn/tex/piet.html</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19990428113621im_/http://dewey.rug.ac.be/barn/tex/cv.html</t>
+  </si>
+  <si>
+    <t>\barn</t>
+  </si>
+  <si>
+    <t>beurs</t>
+  </si>
+  <si>
+    <t>s-miel.gif</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19991104064655im_/http://dewey.rug.ac.be/barn/tex/beurs.html</t>
+  </si>
+  <si>
+    <t>sputnick</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19991104064845im_/http://dewey.rug.ac.be/barn/tex/sputnick.html</t>
   </si>
 </sst>
 </file>
@@ -459,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C76494D-2E19-FC47-898C-1DF4C006E5EB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,82 +561,191 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -562,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0463619A-DD2D-FC46-8005-D86C3722E5D1}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,6 +790,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add various YFCF files
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7812E86E-5B8B-2347-A6BB-747B9225FAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9110B96F-D3D7-4E4B-B069-7EEED2495C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>HTML</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>https://web.archive.org/web/19991104064845im_/http://dewey.rug.ac.be/barn/tex/sputnick.html</t>
+  </si>
+  <si>
+    <t>\YFCF</t>
+  </si>
+  <si>
+    <t>SonicYFCF</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19991104065234im_/http://dewey.rug.ac.be/YFCF/SonicYFCF.html</t>
+  </si>
+  <si>
+    <t>HotSonic</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19991104070439im_/http://dewey.rug.ac.be/YFCF/HotSonic.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19991104070723im_/http://dewey.rug.ac.be/YFCF/UnploughCD.html</t>
+  </si>
+  <si>
+    <t>UnploughCD</t>
   </si>
 </sst>
 </file>
@@ -543,14 +564,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C76494D-2E19-FC47-898C-1DF4C006E5EB}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="86.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -746,6 +768,35 @@
       </c>
       <c r="B27" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing images and movs
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9110B96F-D3D7-4E4B-B069-7EEED2495C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B68258-9BAE-1342-ADC9-B4081E8503BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
@@ -206,23 +206,31 @@
     <t>HotSonic</t>
   </si>
   <si>
-    <t>https://web.archive.org/web/19991104070439im_/http://dewey.rug.ac.be/YFCF/HotSonic.html</t>
-  </si>
-  <si>
     <t>https://web.archive.org/web/19991104070723im_/http://dewey.rug.ac.be/YFCF/UnploughCD.html</t>
   </si>
   <si>
     <t>UnploughCD</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19970719105949/http://dewey.rug.ac.be/YFCF/HotSonic.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,13 +253,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,7 +578,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,19 +798,22 @@
       <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
-        <v>56</v>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B33" r:id="rId1" xr:uid="{9049B73A-964B-954C-A99D-C9F3FE8B8703}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add goodegg and birdflock files
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B68258-9BAE-1342-ADC9-B4081E8503BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4654D852-823F-1540-8617-71B53D60B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>HTML</t>
   </si>
@@ -56,9 +56,6 @@
     <t>video</t>
   </si>
   <si>
-    <t>https://web.archive.org/web/19990428123223im_/http://dewey.rug.ac.be/barn/tex/video.html</t>
-  </si>
-  <si>
     <t>perfo</t>
   </si>
   <si>
@@ -213,6 +210,21 @@
   </si>
   <si>
     <t>https://web.archive.org/web/19970719105949/http://dewey.rug.ac.be/YFCF/HotSonic.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19970715175954im_/http://dewey.rug.ac.be/barn/tex/video.html</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19970719105040im_/http://dewey.rug.ac.be/barn/tex/bird.html</t>
+  </si>
+  <si>
+    <t>goodegg</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19970719105100im_/http://dewey.rug.ac.be/barn/tex/goodegg.html</t>
   </si>
 </sst>
 </file>
@@ -575,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C76494D-2E19-FC47-898C-1DF4C006E5EB}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,14 +606,14 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -617,202 +629,220 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>52</v>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1" xr:uid="{9049B73A-964B-954C-A99D-C9F3FE8B8703}"/>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{9049B73A-964B-954C-A99D-C9F3FE8B8703}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{F3252B96-52B0-CF47-AC7D-300848755EA1}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{E94C0501-F03C-7D43-91CC-79ACE9E0A4EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -836,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -844,23 +874,23 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing media and some fmt edits
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8080E0-4E89-404B-84A0-AF661AB900DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E47CE63-41BE-CF4A-9815-6A0480DA7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="2" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="mementos" sheetId="1" r:id="rId1"/>
+    <sheet name="missing" sheetId="2" r:id="rId2"/>
+    <sheet name="sputnick" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>HTML</t>
   </si>
@@ -92,21 +93,12 @@
     <t>https://web.archive.org/web/19990220051455im_/http://dewey.rug.ac.be/barn/tex/news.html</t>
   </si>
   <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>b-daf.jpeg</t>
-  </si>
-  <si>
     <t>neckprom</t>
   </si>
   <si>
     <t>https://web.archive.org/web/19990501223642im_/http://dewey.rug.ac.be/barn/tex/neckprom.html</t>
   </si>
   <si>
-    <t>b-bertje.jpeg</t>
-  </si>
-  <si>
     <t>gold</t>
   </si>
   <si>
@@ -179,9 +171,6 @@
     <t>beurs</t>
   </si>
   <si>
-    <t>s-miel.gif</t>
-  </si>
-  <si>
     <t>https://web.archive.org/web/19991104064655im_/http://dewey.rug.ac.be/barn/tex/beurs.html</t>
   </si>
   <si>
@@ -225,6 +214,90 @@
   </si>
   <si>
     <t>https://web.archive.org/web/19970719105100im_/http://dewey.rug.ac.be/barn/tex/goodegg.html</t>
+  </si>
+  <si>
+    <t>AUDIO</t>
+  </si>
+  <si>
+    <t>all missing</t>
+  </si>
+  <si>
+    <t>VIDEO</t>
+  </si>
+  <si>
+    <t>archived and downloaded but unsupported format</t>
+  </si>
+  <si>
+    <t>IMAGES</t>
+  </si>
+  <si>
+    <t>none missing</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>memento</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19961120201315/http://syy.oulu.fi/music/</t>
+  </si>
+  <si>
+    <t>http://syy.oulu.fi/music.html</t>
+  </si>
+  <si>
+    <t>http://www.missouri.edu/~uc489745/music.html</t>
+  </si>
+  <si>
+    <t>http://www.yahoo.com/Entertainment/Music/</t>
+  </si>
+  <si>
+    <t>http://www.music.indiana.edu/misc/music_resources.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19981205170619/http://www.music.indiana.edu/misc/music_resources.html</t>
+  </si>
+  <si>
+    <t>http://www.pathfinder.com/@@2k6FXQAAAAAAgAHU/vibe/mmm/music.html</t>
+  </si>
+  <si>
+    <t>http://orpheus.ucsd.edu/webmaster/harmony.html</t>
+  </si>
+  <si>
+    <t>http://www.leeds.ac.uk/music.html</t>
+  </si>
+  <si>
+    <t>http://web.archive.org/web/19961019180127/http://www.leeds.ac.uk/music.html</t>
+  </si>
+  <si>
+    <t>http://harmony-central.mit.edu/</t>
+  </si>
+  <si>
+    <t>http://web.archive.org/web/19961105182741/http://harmony-central.com/</t>
+  </si>
+  <si>
+    <t>became commercial but shows MIT origins</t>
+  </si>
+  <si>
+    <t>http://datura.cerl.uiuc.edu/netstuff/sigsoundLinks.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19971210111447/http://datura.cerl.uiuc.edu/netstuff/sigsoundLinks.html</t>
+  </si>
+  <si>
+    <t>http://datura.cerl.uiuc.edu/schools/courses.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19971210110432/http://datura.cerl.uiuc.edu/schools/courses.html</t>
+  </si>
+  <si>
+    <t>http://american.recordings.com/wwwofmusic/index.html</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/19961227203847/http://ubl.com/</t>
+  </si>
+  <si>
+    <t>became commercial; not sure whether original intent is reflected</t>
   </si>
 </sst>
 </file>
@@ -589,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C76494D-2E19-FC47-898C-1DF4C006E5EB}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +679,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -630,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -683,159 +756,159 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -843,6 +916,7 @@
     <hyperlink ref="B35" r:id="rId1" xr:uid="{9049B73A-964B-954C-A99D-C9F3FE8B8703}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{F3252B96-52B0-CF47-AC7D-300848755EA1}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{E94C0501-F03C-7D43-91CC-79ACE9E0A4EA}"/>
+    <hyperlink ref="B25" r:id="rId4" xr:uid="{02A972B7-FD1A-F645-8015-0CC06D7807DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -850,15 +924,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0463619A-DD2D-FC46-8005-D86C3722E5D1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -866,34 +940,146 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35AF0D3-F9C2-F04A-80C8-FC787D326A87}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="69.33203125" customWidth="1"/>
+    <col min="3" max="3" width="108.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1" xr:uid="{AAD382A2-5B92-CE42-BE68-3FFC84094A2B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uploading more migrated mov files
</commit_message>
<xml_diff>
--- a/barn/urls.xlsx
+++ b/barn/urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbert/Library/CloudStorage/Dropbox/aDisk/yfcf-site/yfcf-site.github.io/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E47CE63-41BE-CF4A-9815-6A0480DA7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821F99C-422F-804D-A222-CA54965A1024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="2" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{8E97D6DA-1012-8849-AB4A-86B743B009B3}"/>
   </bookViews>
   <sheets>
     <sheet name="mementos" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t>HTML</t>
   </si>
@@ -225,9 +225,6 @@
     <t>VIDEO</t>
   </si>
   <si>
-    <t>archived and downloaded but unsupported format</t>
-  </si>
-  <si>
     <t>IMAGES</t>
   </si>
   <si>
@@ -298,6 +295,12 @@
   </si>
   <si>
     <t>became commercial; not sure whether original intent is reflected</t>
+  </si>
+  <si>
+    <t>f-claemit.mov missing</t>
+  </si>
+  <si>
+    <t>f-room.mov missing</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,7 +777,7 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -917,6 +920,7 @@
     <hyperlink ref="B5" r:id="rId2" xr:uid="{F3252B96-52B0-CF47-AC7D-300848755EA1}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{E94C0501-F03C-7D43-91CC-79ACE9E0A4EA}"/>
     <hyperlink ref="B25" r:id="rId4" xr:uid="{02A972B7-FD1A-F645-8015-0CC06D7807DE}"/>
+    <hyperlink ref="B16" r:id="rId5" xr:uid="{3840ED42-BDD3-4B4B-B425-754C6479CB6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -924,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0463619A-DD2D-FC46-8005-D86C3722E5D1}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,15 +944,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -964,7 +968,12 @@
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -976,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35AF0D3-F9C2-F04A-80C8-FC787D326A87}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,97 +997,98 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
         <v>75</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
         <v>77</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
         <v>80</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>85</v>
-      </c>
-      <c r="D13" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" xr:uid="{AAD382A2-5B92-CE42-BE68-3FFC84094A2B}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{FF4986B8-0719-F745-9146-DEA169F272EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>